<commit_message>
edits to read template file
editzz
</commit_message>
<xml_diff>
--- a/db_feed/v6_example.xlsx
+++ b/db_feed/v6_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aliu319\Documents\GitHub\ofet-db\db_feed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\GitHub\ofet-db\db_feed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4409813-1512-4481-BA1B-1B7B7BF754DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3187F537-CA7F-4850-9CD4-9E1952DC7860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F8B411A1-6901-4B9B-966C-09D3D94CB0BB}"/>
+    <workbookView xWindow="2655" yWindow="240" windowWidth="25425" windowHeight="14595" activeTab="4" xr2:uid="{F8B411A1-6901-4B9B-966C-09D3D94CB0BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Origin" sheetId="9" r:id="rId1"/>
@@ -2098,7 +2098,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2429,12 +2429,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2763,7 +2757,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2773,8 +2767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87527978-2A5B-6545-88F5-0DA220A53CEB}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -2782,7 +2776,7 @@
     <col min="1" max="1" width="75.7109375" style="8" customWidth="1"/>
     <col min="2" max="2" width="24" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.85546875" style="8" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="8" customWidth="1"/>
     <col min="5" max="5" width="52.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="8.7109375" style="3"/>
@@ -2802,10 +2796,10 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="37.5" customHeight="1">
-      <c r="A2" s="131" t="s">
+      <c r="A2" s="129" t="s">
         <v>216</v>
       </c>
-      <c r="B2" s="131"/>
+      <c r="B2" s="129"/>
       <c r="C2" s="36"/>
       <c r="D2" s="36"/>
       <c r="E2" s="7"/>
@@ -3191,6 +3185,18 @@
   <mergeCells count="1">
     <mergeCell ref="A2:B2"/>
   </mergeCells>
+  <conditionalFormatting sqref="A5:A8 A11">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A10">
     <cfRule type="colorScale" priority="9">
       <colorScale>
@@ -3215,6 +3221,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A21">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B5:D9">
     <cfRule type="colorScale" priority="14">
       <colorScale>
@@ -3227,8 +3245,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A8 A11">
-    <cfRule type="colorScale" priority="15">
+  <conditionalFormatting sqref="D14:D16">
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3289,30 +3307,6 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="D37:D39">
     <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D14:D16">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A21">
-    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4106,8 +4100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E40DAF9E-DFED-405D-ADE1-B4B8917B7A0A}">
   <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -4135,11 +4129,11 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="104.25" customHeight="1">
-      <c r="A2" s="132" t="s">
+      <c r="A2" s="130" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="133"/>
-      <c r="C2" s="133"/>
+      <c r="B2" s="131"/>
+      <c r="C2" s="131"/>
     </row>
     <row r="4" spans="1:5" ht="15.75">
       <c r="A4" s="96" t="s">
@@ -4216,10 +4210,10 @@
       <c r="A11" s="69" t="s">
         <v>267</v>
       </c>
-      <c r="B11" s="128" t="s">
+      <c r="B11" s="40" t="s">
         <v>278</v>
       </c>
-      <c r="C11" s="129"/>
+      <c r="C11" s="45"/>
       <c r="D11" s="42"/>
     </row>
     <row r="12" spans="1:5">
@@ -4229,7 +4223,7 @@
       <c r="B12" s="123" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="129"/>
+      <c r="C12" s="45"/>
       <c r="D12" s="43"/>
       <c r="E12" t="s">
         <v>68</v>
@@ -4242,7 +4236,7 @@
       <c r="B13" s="51">
         <v>1140</v>
       </c>
-      <c r="C13" s="129"/>
+      <c r="C13" s="45"/>
       <c r="D13" s="43"/>
       <c r="E13" s="35" t="s">
         <v>1</v>
@@ -4255,7 +4249,7 @@
       <c r="B14" s="55">
         <v>1</v>
       </c>
-      <c r="C14" s="130"/>
+      <c r="C14" s="128"/>
       <c r="D14" s="44"/>
       <c r="E14" t="s">
         <v>282</v>
@@ -4636,8 +4630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A6BB566-6734-43D2-B721-97B73307DE8D}">
   <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4664,19 +4658,19 @@
       </c>
       <c r="E1" s="6"/>
       <c r="F1" s="22"/>
-      <c r="G1" s="134" t="s">
+      <c r="G1" s="132" t="s">
         <v>73</v>
       </c>
-      <c r="H1" s="135"/>
-      <c r="I1" s="135"/>
-      <c r="J1" s="136"/>
+      <c r="H1" s="133"/>
+      <c r="I1" s="133"/>
+      <c r="J1" s="134"/>
     </row>
     <row r="2" spans="1:10" ht="130.15" customHeight="1">
-      <c r="A2" s="132" t="s">
+      <c r="A2" s="130" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="133"/>
-      <c r="C2" s="133"/>
+      <c r="B2" s="131"/>
+      <c r="C2" s="131"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="G2" s="3"/>
@@ -5927,9 +5921,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA77467B-0896-49AB-8867-B82D0CAEB0D4}">
   <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L25" sqref="L25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A68" sqref="A68:XFD68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5950,19 +5944,19 @@
         <v>167</v>
       </c>
       <c r="E1" s="38"/>
-      <c r="G1" s="134" t="s">
+      <c r="G1" s="132" t="s">
         <v>73</v>
       </c>
-      <c r="H1" s="135"/>
-      <c r="I1" s="135"/>
-      <c r="J1" s="136"/>
+      <c r="H1" s="133"/>
+      <c r="I1" s="133"/>
+      <c r="J1" s="134"/>
     </row>
     <row r="2" spans="1:10" ht="130.5" customHeight="1">
-      <c r="A2" s="132" t="s">
+      <c r="A2" s="130" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="133"/>
-      <c r="C2" s="133"/>
+      <c r="B2" s="131"/>
+      <c r="C2" s="131"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -6714,19 +6708,19 @@
       <c r="D1" t="s">
         <v>167</v>
       </c>
-      <c r="F1" s="134" t="s">
+      <c r="F1" s="132" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="135"/>
-      <c r="H1" s="135"/>
-      <c r="I1" s="136"/>
+      <c r="G1" s="133"/>
+      <c r="H1" s="133"/>
+      <c r="I1" s="134"/>
     </row>
     <row r="2" spans="1:10" ht="93" customHeight="1">
-      <c r="A2" s="132" t="s">
+      <c r="A2" s="130" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="133"/>
-      <c r="C2" s="133"/>
+      <c r="B2" s="131"/>
+      <c r="C2" s="131"/>
       <c r="D2" s="52"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -7304,7 +7298,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{407D2B8A-E356-4CF8-BF78-D6DBB98A494F}">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -7328,19 +7322,19 @@
         <v>167</v>
       </c>
       <c r="E1" s="38"/>
-      <c r="G1" s="134" t="s">
+      <c r="G1" s="132" t="s">
         <v>73</v>
       </c>
-      <c r="H1" s="135"/>
-      <c r="I1" s="135"/>
-      <c r="J1" s="136"/>
+      <c r="H1" s="133"/>
+      <c r="I1" s="133"/>
+      <c r="J1" s="134"/>
     </row>
     <row r="2" spans="1:10" ht="129.75" customHeight="1">
-      <c r="A2" s="132" t="s">
+      <c r="A2" s="130" t="s">
         <v>192</v>
       </c>
-      <c r="B2" s="133"/>
-      <c r="C2" s="133"/>
+      <c r="B2" s="131"/>
+      <c r="C2" s="131"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -7684,7 +7678,7 @@
   <dimension ref="A1:O55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15"/>
@@ -7721,12 +7715,12 @@
         <v>167</v>
       </c>
       <c r="H1"/>
-      <c r="I1" s="134" t="s">
+      <c r="I1" s="132" t="s">
         <v>73</v>
       </c>
-      <c r="J1" s="135"/>
-      <c r="K1" s="135"/>
-      <c r="L1" s="136"/>
+      <c r="J1" s="133"/>
+      <c r="K1" s="133"/>
+      <c r="L1" s="134"/>
     </row>
     <row r="2" spans="1:15" s="8" customFormat="1" ht="15.75">
       <c r="A2" s="57" t="s">
@@ -8736,20 +8730,20 @@
       <c r="G1" t="s">
         <v>167</v>
       </c>
-      <c r="I1" s="134" t="s">
+      <c r="I1" s="132" t="s">
         <v>73</v>
       </c>
-      <c r="J1" s="135"/>
-      <c r="K1" s="135"/>
-      <c r="L1" s="135"/>
-      <c r="M1" s="136"/>
+      <c r="J1" s="133"/>
+      <c r="K1" s="133"/>
+      <c r="L1" s="133"/>
+      <c r="M1" s="134"/>
     </row>
     <row r="2" spans="1:1020 1028:2044 2052:3068 3076:4092 4100:5116 5124:6140 6148:7164 7172:8188 8196:9212 9220:10236 10244:11260 11268:12284 12292:13308 13316:14332 14340:15356 15364:16380" s="8" customFormat="1" ht="90" customHeight="1">
-      <c r="A2" s="131" t="s">
+      <c r="A2" s="129" t="s">
         <v>384</v>
       </c>
-      <c r="B2" s="131"/>
-      <c r="C2" s="131"/>
+      <c r="B2" s="129"/>
+      <c r="C2" s="129"/>
       <c r="D2" s="13"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>

</xml_diff>